<commit_message>
27 sorting algo add
</commit_message>
<xml_diff>
--- a/hw4/homework_27/datastructure_27.xlsx
+++ b/hw4/homework_27/datastructure_27.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kounuki/data_structure/data_structure_HW/hw4/homework_27/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BBF18A1-20E0-EE43-8184-D3E012924240}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E9B4A6-EB68-9046-8E5C-DA6AAF951DB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{3591628D-1D6F-7748-8256-BF774425804D}"/>
   </bookViews>
@@ -3410,7 +3410,7 @@
   <dimension ref="B5:AA18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20:AF20"/>
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>